<commit_message>
Add CN gdp data and data cleaner
</commit_message>
<xml_diff>
--- a/app/db/mapping/gdp/gdp_mapping_template.xlsx
+++ b/app/db/mapping/gdp/gdp_mapping_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/Interactive_Dashboard/db/mapping/gdp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/econ-db/app/db/mapping/gdp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A013F5-1882-5A4C-988D-4FCCB298E410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95E5E85-9607-F843-A1F0-F72FDE89F4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19080" windowHeight="17500" xr2:uid="{1B2CF28C-13C3-A848-9CC6-2F6227EB377C}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{1B2CF28C-13C3-A848-9CC6-2F6227EB377C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -726,14 +726,15 @@
   <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finish GDP matcher and finish matching
</commit_message>
<xml_diff>
--- a/app/db/mapping/gdp/gdp_mapping_template.xlsx
+++ b/app/db/mapping/gdp/gdp_mapping_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/econ-db/app/db/mapping/gdp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95E5E85-9607-F843-A1F0-F72FDE89F4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD75E1D-70DE-8646-A95A-DB93E466381B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{1B2CF28C-13C3-A848-9CC6-2F6227EB377C}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1B2CF28C-13C3-A848-9CC6-2F6227EB377C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="101">
   <si>
     <t>By expenditure</t>
   </si>
@@ -187,9 +187,6 @@
     <t>USD, % QoQ</t>
   </si>
   <si>
-    <t>% of GDP</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Total</t>
   </si>
   <si>
@@ -338,6 +335,12 @@
   </si>
   <si>
     <t>LCU, Contribution to % QoQ chg, ppts</t>
+  </si>
+  <si>
+    <t>LCU, % of GDP</t>
+  </si>
+  <si>
+    <t>LCU, % of GDP, SA</t>
   </si>
 </sst>
 </file>
@@ -726,7 +729,7 @@
   <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,7 +748,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
         <v>36</v>
@@ -756,7 +759,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -770,7 +773,7 @@
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -801,7 +804,7 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -837,7 +840,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -848,7 +851,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -859,10 +862,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -870,7 +873,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
@@ -881,10 +884,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -892,10 +895,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>6</v>
@@ -903,10 +906,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -914,10 +917,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <v>6</v>
@@ -925,72 +928,75 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
       <c r="C17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="D19">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D22">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
@@ -998,15 +1004,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1022,41 +1028,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="D32">
         <v>7</v>
@@ -1064,7 +1070,7 @@
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D33">
         <v>7</v>
@@ -1072,7 +1078,7 @@
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34">
         <v>7</v>
@@ -1080,7 +1086,7 @@
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D35">
         <v>6</v>
@@ -1088,7 +1094,7 @@
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36">
         <v>6</v>
@@ -1096,7 +1102,7 @@
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D37">
         <v>6</v>
@@ -1104,7 +1110,7 @@
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C38" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38">
         <v>6</v>
@@ -1112,7 +1118,7 @@
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D39">
         <v>7</v>
@@ -1120,7 +1126,7 @@
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40">
         <v>8</v>
@@ -1128,7 +1134,7 @@
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D41">
         <v>8</v>
@@ -1136,7 +1142,7 @@
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C42" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D42">
         <v>8</v>
@@ -1144,7 +1150,7 @@
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D43">
         <v>8</v>
@@ -1152,7 +1158,7 @@
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C44" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44">
         <v>7</v>
@@ -1160,7 +1166,7 @@
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D45">
         <v>7</v>
@@ -1168,7 +1174,7 @@
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C46" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D46">
         <v>7</v>
@@ -1176,7 +1182,7 @@
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C47" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D47">
         <v>6</v>
@@ -1184,7 +1190,7 @@
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C48" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D48">
         <v>7</v>
@@ -1192,7 +1198,7 @@
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D49">
         <v>8</v>
@@ -1200,7 +1206,7 @@
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C50" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D50">
         <v>8</v>
@@ -1208,7 +1214,7 @@
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C51" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D51">
         <v>8</v>
@@ -1216,7 +1222,7 @@
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C52" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D52">
         <v>8</v>
@@ -1224,7 +1230,7 @@
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C53" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D53">
         <v>7</v>
@@ -1232,7 +1238,7 @@
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D54">
         <v>7</v>
@@ -1240,7 +1246,7 @@
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C55" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D55">
         <v>7</v>
@@ -1256,7 +1262,7 @@
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C57" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D57">
         <v>6</v>
@@ -1264,7 +1270,7 @@
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C58" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D58">
         <v>6</v>
@@ -1272,7 +1278,7 @@
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C59" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59">
         <v>6</v>
@@ -1280,7 +1286,7 @@
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D60">
         <v>3</v>
@@ -1288,7 +1294,7 @@
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D61">
         <v>4</v>
@@ -1296,7 +1302,7 @@
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D62">
         <v>4</v>
@@ -1304,7 +1310,7 @@
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D63">
         <v>5</v>
@@ -1328,7 +1334,7 @@
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D66">
         <v>4</v>
@@ -1336,7 +1342,7 @@
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D67">
         <v>5</v>

</xml_diff>

<commit_message>
all new options for japan added, new gdp data added for all countries but some might be missing options
</commit_message>
<xml_diff>
--- a/app/db/mapping/gdp/gdp_mapping_template.xlsx
+++ b/app/db/mapping/gdp/gdp_mapping_template.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$C$1:$D$107</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$C$1:$D$162</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="160">
   <si>
     <t>Main_category</t>
   </si>
@@ -42,100 +42,118 @@
     <t>USD</t>
   </si>
   <si>
+    <t>Per capita</t>
+  </si>
+  <si>
+    <t>RGDP Q</t>
+  </si>
+  <si>
+    <t>LCU, % YoY</t>
+  </si>
+  <si>
     <t>GDP</t>
   </si>
   <si>
-    <t>RGDP Q</t>
-  </si>
-  <si>
-    <t>LCU, % YoY</t>
+    <t>RGDP A</t>
+  </si>
+  <si>
+    <t>USD, % YoY</t>
   </si>
   <si>
     <t>Domestic Demand</t>
   </si>
   <si>
-    <t>RGDP A</t>
-  </si>
-  <si>
-    <t>USD, % YoY</t>
+    <t>GDP deflator</t>
+  </si>
+  <si>
+    <t>LCU, % QoQ</t>
   </si>
   <si>
     <t xml:space="preserve">  Per capita</t>
   </si>
   <si>
-    <t>GDP deflator</t>
-  </si>
-  <si>
-    <t>LCU, % QoQ</t>
+    <t>Deflator A</t>
+  </si>
+  <si>
+    <t>USD, % QoQ</t>
   </si>
   <si>
     <t xml:space="preserve">  Total</t>
   </si>
   <si>
-    <t>Deflator A</t>
-  </si>
-  <si>
-    <t>USD, % QoQ</t>
+    <t>LCU, Contribution to % YoY chg, ppts</t>
   </si>
   <si>
     <t xml:space="preserve">  Private</t>
   </si>
   <si>
-    <t>LCU, Contribution to % YoY chg, ppts</t>
+    <t>LCU, Contribution to % QoQ chg, ppts</t>
   </si>
   <si>
     <t xml:space="preserve">  Public</t>
   </si>
   <si>
-    <t>LCU, Contribution to % QoQ chg, ppts</t>
+    <t>LCU, % of GDP</t>
   </si>
   <si>
     <t xml:space="preserve">  Government Consumption</t>
   </si>
   <si>
-    <t>LCU, % of GDP</t>
+    <t>LCU, % of GDP, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Employee compensation per hour</t>
+  </si>
+  <si>
+    <t>LCU, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Employee compensation per worker</t>
+  </si>
+  <si>
+    <t>USD, SA</t>
   </si>
   <si>
     <t xml:space="preserve">  Private Consumption</t>
   </si>
   <si>
-    <t>LCU, % of GDP, SA</t>
+    <t>LCU, % YoY, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Per capita</t>
+  </si>
+  <si>
+    <t>USD, % YoY, SA</t>
   </si>
   <si>
     <t xml:space="preserve">     Total</t>
   </si>
   <si>
-    <t>LCU, SA</t>
+    <t>LCU, % QoQ, SA</t>
   </si>
   <si>
     <t xml:space="preserve">     Excluding Imputed Rent</t>
   </si>
   <si>
-    <t>USD, SA</t>
+    <t>USD, % QoQ, SA</t>
   </si>
   <si>
     <t xml:space="preserve">     Household Consumption</t>
   </si>
   <si>
-    <t>LCU, % YoY, SA</t>
+    <t xml:space="preserve">        Per capita</t>
   </si>
   <si>
     <t xml:space="preserve">        Total</t>
   </si>
   <si>
-    <t>USD, % YoY, SA</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Direct Purchases Abroad by Resident Households</t>
   </si>
   <si>
-    <t>LCU, % QoQ, SA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Direct Purchases in the Domestic Market by Non-Resident Households </t>
-  </si>
-  <si>
-    <t>USD, % QoQ, SA</t>
+    <t xml:space="preserve">        Direct Purchases in the Domestic Market by Non-Resident Households </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Excluding Imputed Rent</t>
   </si>
   <si>
     <t xml:space="preserve">        Domestic Final Consumption</t>
@@ -171,12 +189,21 @@
     <t xml:space="preserve">    Private</t>
   </si>
   <si>
+    <t xml:space="preserve">      Inventories</t>
+  </si>
+  <si>
     <t xml:space="preserve">    Public</t>
   </si>
   <si>
     <t xml:space="preserve">    Gross Fixed Capital Formation</t>
   </si>
   <si>
+    <t xml:space="preserve">      Buildings and Structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Residential</t>
+  </si>
+  <si>
     <t xml:space="preserve">      Total</t>
   </si>
   <si>
@@ -207,6 +234,9 @@
     <t xml:space="preserve">      Private</t>
   </si>
   <si>
+    <t xml:space="preserve">        Non-Residential</t>
+  </si>
+  <si>
     <t xml:space="preserve">        Construction</t>
   </si>
   <si>
@@ -339,6 +369,15 @@
     <t xml:space="preserve">  Secondary</t>
   </si>
   <si>
+    <t xml:space="preserve">      Electronic components and devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fabricated metal products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Basic metal</t>
+  </si>
+  <si>
     <t xml:space="preserve">      Food products and beverages</t>
   </si>
   <si>
@@ -360,14 +399,107 @@
     <t xml:space="preserve">      Non-metallic mineral products</t>
   </si>
   <si>
-    <t xml:space="preserve">      Fabricated metal products</t>
+    <t xml:space="preserve">      General-purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        production and business oriented machinery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Electrical machinery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        equipment and supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Information and communication electronics equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Transport equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Other manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      gas and water supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        waste management service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tertiary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Wholesale and retail trade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Transport and postal services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Accommodation and food services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Information and communications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Finance and insurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Real estate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Professional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      scientific and technical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Public administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Human health and social work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sub-total</t>
+  </si>
+  <si>
+    <t>Households</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Saving ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  NGDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Per capita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RGDI</t>
+  </si>
+  <si>
+    <t>HP filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  trend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  output gap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -385,6 +517,11 @@
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -430,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -439,12 +576,21 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -705,10 +851,10 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>3.0</v>
       </c>
     </row>
@@ -733,11 +879,11 @@
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -747,7 +893,7 @@
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="1">
@@ -794,7 +940,7 @@
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="1">
@@ -808,8 +954,8 @@
       <c r="C11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1">
-        <v>5.0</v>
+      <c r="D11" s="3">
+        <v>4.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -819,41 +965,41 @@
       <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="1">
-        <v>5.0</v>
+      <c r="D12" s="3">
+        <v>4.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="1">
-        <v>6.0</v>
+      <c r="D14" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -864,70 +1010,70 @@
         <v>39</v>
       </c>
       <c r="D16" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="C18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="3">
         <v>6.0</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="C18" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="1">
-        <v>7.0</v>
-      </c>
-    </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="1">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="1">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="1">
-        <v>8.0</v>
+      <c r="D22" s="3">
+        <v>6.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="1">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="1">
@@ -935,167 +1081,167 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D25" s="1">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D26" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="C31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="C32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="C33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="C34" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="3">
         <v>6.0</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="1">
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="C35" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="C36" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="3">
         <v>6.0</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="1">
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="C37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="C38" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="C39" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="3">
         <v>7.0</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="1">
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="C40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="C41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="C42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="1">
         <v>7.0</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="1">
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="C43" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="1">
         <v>7.0</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="1">
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="C44" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="1">
         <v>7.0</v>
       </c>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="1">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D45" s="1">
@@ -1103,23 +1249,23 @@
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="5" t="s">
         <v>69</v>
       </c>
       <c r="D46" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="5" t="s">
         <v>70</v>
       </c>
       <c r="D47" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D48" s="1">
@@ -1127,200 +1273,200 @@
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="4" t="s">
-        <v>64</v>
+      <c r="C49" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="D49" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="C50" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="3">
         <v>7.0</v>
       </c>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D50" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="1">
-        <v>8.0</v>
+      <c r="C51" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="3">
+        <v>7.0</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="4" t="s">
-        <v>66</v>
+      <c r="C52" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="D52" s="1">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="4" t="s">
-        <v>67</v>
+      <c r="C53" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D53" s="1">
         <v>8.0</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="4" t="s">
-        <v>68</v>
+      <c r="C54" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="D54" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="C55" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="C56" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="C57" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="1">
         <v>7.0</v>
       </c>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D55" s="1">
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="C58" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58" s="1">
         <v>7.0</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D56" s="1">
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="C59" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" s="1">
         <v>7.0</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D58" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="6" t="s">
-        <v>74</v>
+      <c r="C60" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D60" s="1">
         <v>6.0</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="C62" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="C63" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D61" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="C64" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D63" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D64" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D65" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D66" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D67" s="1">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="1" t="s">
-        <v>50</v>
+      <c r="C68" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="D68" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="C69" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D69" s="1">
         <v>5.0</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="1" t="s">
-        <v>78</v>
+      <c r="C70" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="D70" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="2" t="s">
-        <v>80</v>
+      <c r="C71" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="D71" s="1">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="1" t="s">
-        <v>81</v>
+      <c r="C72" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="D72" s="1">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="C73" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D73" s="1">
         <v>3.0</v>
@@ -1328,15 +1474,15 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="C74" s="1" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="D74" s="1">
         <v>4.0</v>
       </c>
     </row>
-    <row r="75" ht="15.0" customHeight="1">
+    <row r="75" ht="15.75" customHeight="1">
       <c r="C75" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D75" s="1">
         <v>4.0</v>
@@ -1344,31 +1490,31 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="C76" s="1" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="D76" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="C77" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D77" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="C78" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D78" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="C79" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D79" s="1">
         <v>4.0</v>
@@ -1376,55 +1522,55 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="C80" s="1" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="D80" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="81" ht="15.75" customHeight="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="81" ht="15.0" customHeight="1">
       <c r="C81" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D81" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="C82" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D82" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="1" t="s">
-        <v>92</v>
+      <c r="C83" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D83" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="C84" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D84" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="C85" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D85" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="C86" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D86" s="1">
         <v>4.0</v>
@@ -1432,7 +1578,7 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="C87" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D87" s="1">
         <v>4.0</v>
@@ -1440,7 +1586,7 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="C88" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D88" s="1">
         <v>4.0</v>
@@ -1448,7 +1594,7 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="C89" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D89" s="1">
         <v>4.0</v>
@@ -1456,7 +1602,7 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="C90" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D90" s="1">
         <v>4.0</v>
@@ -1464,7 +1610,7 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="C91" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D91" s="1">
         <v>4.0</v>
@@ -1472,187 +1618,572 @@
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="C92" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D92" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="93" ht="15.75" customHeight="1">
+      <c r="C93" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D93" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="94" ht="15.75" customHeight="1">
+      <c r="C94" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D92" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="7" t="s">
+      <c r="D94" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="95" ht="15.75" customHeight="1">
+      <c r="C95" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D95" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="96" ht="15.75" customHeight="1">
+      <c r="C96" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D96" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="97" ht="15.75" customHeight="1">
+      <c r="C97" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D97" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="98" ht="15.75" customHeight="1">
+      <c r="C98" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D98" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="99" ht="15.75" customHeight="1">
+      <c r="C99" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D99" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="100" ht="15.75" customHeight="1">
+      <c r="C100" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D100" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="101" ht="15.75" customHeight="1">
+      <c r="C101" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D101" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="102" ht="15.75" customHeight="1">
+      <c r="C102" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D102" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="103" ht="15.75" customHeight="1">
+      <c r="C103" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D103" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="104" ht="15.75" customHeight="1">
+      <c r="C104" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D104" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="105" ht="15.75" customHeight="1">
+      <c r="C105" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D105" s="1">
         <v>2.0</v>
-      </c>
-    </row>
-    <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D94" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D95" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D96" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D97" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D98" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D99" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D100" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D101" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D102" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D103" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D104" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D105" s="3">
-        <v>5.0</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="C106" s="3" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="D106" s="3">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="C107" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D107" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="108" ht="15.75" customHeight="1">
+      <c r="C108" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D108" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="109" ht="15.75" customHeight="1">
+      <c r="C109" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D109" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="110" ht="15.75" customHeight="1">
+      <c r="C110" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D107" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
+      <c r="D110" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="111" ht="15.75" customHeight="1">
+      <c r="C111" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D111" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="112" ht="15.75" customHeight="1">
+      <c r="C112" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D112" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="113" ht="15.75" customHeight="1">
+      <c r="C113" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D113" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="114" ht="15.75" customHeight="1">
+      <c r="C114" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D114" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="115" ht="15.75" customHeight="1">
+      <c r="C115" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D115" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="116" ht="15.75" customHeight="1">
+      <c r="C116" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D116" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="117" ht="15.75" customHeight="1">
+      <c r="C117" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D117" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="118" ht="15.75" customHeight="1">
+      <c r="C118" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D118" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="119" ht="15.75" customHeight="1">
+      <c r="C119" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D119" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="120" ht="15.75" customHeight="1">
+      <c r="C120" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D120" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="121" ht="15.75" customHeight="1">
+      <c r="C121" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D121" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="122" ht="15.75" customHeight="1">
+      <c r="C122" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D122" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="123" ht="15.75" customHeight="1">
+      <c r="C123" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D123" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="124" ht="15.75" customHeight="1">
+      <c r="C124" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D124" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="125" ht="15.75" customHeight="1">
+      <c r="C125" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D125" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="126" ht="15.75" customHeight="1">
+      <c r="C126" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D126" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="127" ht="15.75" customHeight="1">
+      <c r="C127" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D127" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="128" ht="15.75" customHeight="1">
+      <c r="C128" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D128" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="129" ht="15.75" customHeight="1">
+      <c r="C129" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D129" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="130" ht="15.75" customHeight="1">
+      <c r="C130" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D130" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="131" ht="15.75" customHeight="1">
+      <c r="C131" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D131" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="132" ht="15.75" customHeight="1">
+      <c r="C132" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D132" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="133" ht="15.75" customHeight="1">
+      <c r="C133" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D133" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="134" ht="15.75" customHeight="1">
+      <c r="C134" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D134" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="135" ht="15.75" customHeight="1">
+      <c r="C135" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D135" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="136" ht="15.75" customHeight="1">
+      <c r="C136" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D136" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="137" ht="15.75" customHeight="1">
+      <c r="C137" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D137" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="138" ht="15.75" customHeight="1">
+      <c r="C138" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D138" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="139" ht="15.75" customHeight="1">
+      <c r="C139" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D139" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="140" ht="15.75" customHeight="1">
+      <c r="C140" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D140" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="141" ht="15.75" customHeight="1">
+      <c r="C141" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D141" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="142" ht="15.75" customHeight="1">
+      <c r="C142" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D142" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="143" ht="15.75" customHeight="1">
+      <c r="C143" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D143" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="144" ht="15.75" customHeight="1">
+      <c r="C144" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D144" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="145" ht="15.75" customHeight="1">
+      <c r="C145" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D145" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="146" ht="15.75" customHeight="1">
+      <c r="C146" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D146" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="147" ht="15.75" customHeight="1">
+      <c r="C147" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D147" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="148" ht="15.75" customHeight="1">
+      <c r="C148" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D148" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="149" ht="15.75" customHeight="1">
+      <c r="C149" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D149" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="150" ht="15.75" customHeight="1">
+      <c r="C150" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D150" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="151" ht="15.75" customHeight="1">
+      <c r="C151" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D151" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="152" ht="15.75" customHeight="1">
+      <c r="C152" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D152" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="153" ht="15.75" customHeight="1">
+      <c r="C153" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D153" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="154" ht="15.75" customHeight="1">
+      <c r="C154" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D154" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="155" ht="15.75" customHeight="1">
+      <c r="C155" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D155" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="156" ht="15.75" customHeight="1">
+      <c r="C156" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D156" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="157" ht="15.75" customHeight="1">
+      <c r="C157" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D157" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="158" ht="15.75" customHeight="1">
+      <c r="C158" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D158" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="159" ht="15.75" customHeight="1">
+      <c r="C159" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D159" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="160" ht="15.75" customHeight="1">
+      <c r="C160" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D160" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="161" ht="15.75" customHeight="1">
+      <c r="C161" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D161" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="162" ht="15.75" customHeight="1">
+      <c r="C162" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D162" s="3">
+        <v>3.0</v>
+      </c>
+    </row>
     <row r="163" ht="15.75" customHeight="1"/>
     <row r="164" ht="15.75" customHeight="1"/>
     <row r="165" ht="15.75" customHeight="1"/>
@@ -2491,8 +3022,23 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="$C$1:$D$107"/>
+  <autoFilter ref="$C$1:$D$162"/>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Frequency select changed to only display a frequency value with Nominal/Real/Deflator now in a new Sector select
</commit_message>
<xml_diff>
--- a/app/db/mapping/gdp/gdp_mapping_template.xlsx
+++ b/app/db/mapping/gdp/gdp_mapping_template.xlsx
@@ -63,7 +63,7 @@
     <t>Domestic Demand</t>
   </si>
   <si>
-    <t>GDP deflator</t>
+    <t>GDP deflator Q</t>
   </si>
   <si>
     <t>LCU, % QoQ</t>
@@ -72,7 +72,7 @@
     <t xml:space="preserve">  Per capita</t>
   </si>
   <si>
-    <t>Deflator A</t>
+    <t>GDP deflator A</t>
   </si>
   <si>
     <t>USD, % QoQ</t>
@@ -901,7 +901,7 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">

</xml_diff>

<commit_message>
fixed the b'' option in selects problem
</commit_message>
<xml_diff>
--- a/app/db/mapping/gdp/gdp_mapping_template.xlsx
+++ b/app/db/mapping/gdp/gdp_mapping_template.xlsx
@@ -499,7 +499,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -519,21 +519,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="12.0"/>
@@ -541,33 +526,21 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -577,20 +550,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -851,7 +810,7 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3">
@@ -893,7 +852,7 @@
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="1">
@@ -951,7 +910,7 @@
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="3">
@@ -962,7 +921,7 @@
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="3">
@@ -973,7 +932,7 @@
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="1">
@@ -984,7 +943,7 @@
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="3">
@@ -995,7 +954,7 @@
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="1">
@@ -1006,7 +965,7 @@
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="1">
@@ -1017,7 +976,7 @@
       <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="1">
@@ -1025,7 +984,7 @@
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="3">
@@ -1033,7 +992,7 @@
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="1">
@@ -1041,7 +1000,7 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="1">
@@ -1049,7 +1008,7 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="1">
@@ -1057,7 +1016,7 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D22" s="3">
@@ -1065,7 +1024,7 @@
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="1">
@@ -1073,7 +1032,7 @@
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="1">
@@ -1081,7 +1040,7 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D25" s="1">
@@ -1089,7 +1048,7 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D26" s="1">
@@ -1097,7 +1056,7 @@
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="1">
@@ -1105,7 +1064,7 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="1">
@@ -1113,7 +1072,7 @@
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="1">
@@ -1121,7 +1080,7 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="1">
@@ -1129,7 +1088,7 @@
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D31" s="1">
@@ -1137,7 +1096,7 @@
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D32" s="1">
@@ -1145,7 +1104,7 @@
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D33" s="1">
@@ -1153,7 +1112,7 @@
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D34" s="3">
@@ -1161,7 +1120,7 @@
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D35" s="1">
@@ -1169,7 +1128,7 @@
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D36" s="3">
@@ -1177,7 +1136,7 @@
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D37" s="1">
@@ -1185,7 +1144,7 @@
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D38" s="3">
@@ -1193,7 +1152,7 @@
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D39" s="3">
@@ -1201,7 +1160,7 @@
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D40" s="1">
@@ -1209,7 +1168,7 @@
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D41" s="1">
@@ -1217,7 +1176,7 @@
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D42" s="1">
@@ -1225,7 +1184,7 @@
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D43" s="1">
@@ -1233,7 +1192,7 @@
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D44" s="1">
@@ -1241,7 +1200,7 @@
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D45" s="1">
@@ -1249,7 +1208,7 @@
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D46" s="1">
@@ -1257,7 +1216,7 @@
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D47" s="1">
@@ -1265,7 +1224,7 @@
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D48" s="1">
@@ -1273,7 +1232,7 @@
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="1">
@@ -1281,7 +1240,7 @@
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D50" s="3">
@@ -1289,7 +1248,7 @@
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D51" s="3">
@@ -1297,7 +1256,7 @@
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D52" s="1">
@@ -1305,7 +1264,7 @@
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D53" s="1">
@@ -1313,7 +1272,7 @@
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D54" s="1">
@@ -1321,7 +1280,7 @@
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D55" s="1">
@@ -1329,7 +1288,7 @@
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D56" s="1">
@@ -1337,7 +1296,7 @@
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D57" s="1">
@@ -1345,7 +1304,7 @@
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D58" s="1">
@@ -1353,7 +1312,7 @@
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D59" s="1">
@@ -1361,7 +1320,7 @@
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D60" s="1">
@@ -1369,7 +1328,7 @@
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D61" s="1">
@@ -1377,7 +1336,7 @@
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D62" s="1">
@@ -1385,7 +1344,7 @@
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D63" s="1">
@@ -1393,7 +1352,7 @@
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D64" s="1">
@@ -1401,7 +1360,7 @@
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D65" s="1">
@@ -1409,7 +1368,7 @@
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D66" s="1">
@@ -1417,7 +1376,7 @@
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D67" s="1">
@@ -1425,7 +1384,7 @@
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D68" s="1">
@@ -1441,7 +1400,7 @@
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D70" s="1">
@@ -1449,7 +1408,7 @@
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="9" t="s">
+      <c r="C71" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D71" s="1">
@@ -1457,7 +1416,7 @@
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D72" s="1">
@@ -1545,7 +1504,7 @@
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="1" t="s">
         <v>90</v>
       </c>
       <c r="D83" s="1">
@@ -1721,7 +1680,7 @@
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="10" t="s">
+      <c r="C105" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D105" s="1">
@@ -1729,7 +1688,7 @@
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="3" t="s">
+      <c r="C106" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D106" s="3">
@@ -1737,7 +1696,7 @@
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="3" t="s">
+      <c r="C107" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D107" s="3">
@@ -1745,7 +1704,7 @@
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="3" t="s">
+      <c r="C108" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D108" s="3">
@@ -1753,7 +1712,7 @@
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="3" t="s">
+      <c r="C109" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D109" s="3">
@@ -1761,7 +1720,7 @@
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="3" t="s">
+      <c r="C110" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D110" s="3">
@@ -1769,7 +1728,7 @@
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="3" t="s">
+      <c r="C111" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D111" s="3">
@@ -1777,7 +1736,7 @@
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="1" t="s">
         <v>117</v>
       </c>
       <c r="D112" s="3">
@@ -1785,7 +1744,7 @@
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="3" t="s">
+      <c r="C113" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D113" s="3">
@@ -1793,7 +1752,7 @@
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="3" t="s">
+      <c r="C114" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D114" s="3">
@@ -1801,7 +1760,7 @@
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="3" t="s">
+      <c r="C115" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D115" s="3">
@@ -1809,7 +1768,7 @@
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="3" t="s">
+      <c r="C116" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D116" s="3">
@@ -1817,7 +1776,7 @@
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="3" t="s">
+      <c r="C117" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D117" s="3">
@@ -1825,7 +1784,7 @@
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="3" t="s">
+      <c r="C118" s="1" t="s">
         <v>120</v>
       </c>
       <c r="D118" s="3">
@@ -1833,7 +1792,7 @@
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="3" t="s">
+      <c r="C119" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D119" s="3">
@@ -1841,7 +1800,7 @@
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="3" t="s">
+      <c r="C120" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D120" s="3">
@@ -1849,7 +1808,7 @@
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="3" t="s">
+      <c r="C121" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D121" s="3">
@@ -1857,7 +1816,7 @@
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="3" t="s">
+      <c r="C122" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D122" s="3">
@@ -1865,7 +1824,7 @@
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="3" t="s">
+      <c r="C123" s="1" t="s">
         <v>125</v>
       </c>
       <c r="D123" s="3">
@@ -1873,7 +1832,7 @@
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="3" t="s">
+      <c r="C124" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D124" s="3">
@@ -1881,7 +1840,7 @@
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="3" t="s">
+      <c r="C125" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D125" s="3">
@@ -1889,7 +1848,7 @@
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="3" t="s">
+      <c r="C126" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D126" s="3">
@@ -1897,7 +1856,7 @@
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="3" t="s">
+      <c r="C127" s="1" t="s">
         <v>128</v>
       </c>
       <c r="D127" s="3">
@@ -1905,7 +1864,7 @@
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="3" t="s">
+      <c r="C128" s="1" t="s">
         <v>129</v>
       </c>
       <c r="D128" s="3">
@@ -2105,7 +2064,7 @@
       </c>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="10" t="s">
+      <c r="C153" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D153" s="1">
@@ -2153,7 +2112,7 @@
       </c>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="10" t="s">
+      <c r="C159" s="4" t="s">
         <v>156</v>
       </c>
       <c r="D159" s="1">

</xml_diff>

<commit_message>
new japanese data, app functionality improved
</commit_message>
<xml_diff>
--- a/app/db/mapping/gdp/gdp_mapping_template.xlsx
+++ b/app/db/mapping/gdp/gdp_mapping_template.xlsx
@@ -63,7 +63,7 @@
     <t>Domestic Demand</t>
   </si>
   <si>
-    <t>GDP deflator Q</t>
+    <t>Deflator Q</t>
   </si>
   <si>
     <t>LCU, % QoQ</t>
@@ -72,7 +72,7 @@
     <t xml:space="preserve">  Per capita</t>
   </si>
   <si>
-    <t>GDP deflator A</t>
+    <t>Deflator A</t>
   </si>
   <si>
     <t>USD, % QoQ</t>

</xml_diff>

<commit_message>
template updates and table/graph fixes
</commit_message>
<xml_diff>
--- a/app/db/mapping/gdp/gdp_mapping_template.xlsx
+++ b/app/db/mapping/gdp/gdp_mapping_template.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$C$1:$D$162</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$C$1:$D$130</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="132">
   <si>
     <t>Main_category</t>
   </si>
@@ -33,7 +33,7 @@
     <t>LCU</t>
   </si>
   <si>
-    <t>By expenditure</t>
+    <t>Expenditure</t>
   </si>
   <si>
     <t>NGDP A</t>
@@ -285,180 +285,123 @@
     <t xml:space="preserve">  Imports of Goods and Services</t>
   </si>
   <si>
-    <t>By industry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Agriculture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Industry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Mining and Quarrying</t>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Primary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Agriculture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      forestry and fishing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Mining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Secondary</t>
   </si>
   <si>
     <t xml:space="preserve">    Manufacturing</t>
   </si>
   <si>
-    <t xml:space="preserve">    Electricity and Gas Supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Water Supply and Remediation Activities</t>
+    <t xml:space="preserve">      Electronic components and devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Fabricated metal products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Basic metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Food products and beverages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Textile products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Pulp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        paper and paper products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Chemicals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Petroleum and coal products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Non-metallic mineral products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      General-purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        production and business oriented machinery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Electrical machinery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        equipment and supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Information and communication electronics equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Transport equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Other manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      gas and water supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        waste management service</t>
   </si>
   <si>
     <t xml:space="preserve">    Construction</t>
   </si>
   <si>
-    <t xml:space="preserve">   Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Wholesale and Retail Trade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Transportation and Storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Accommodation and Food Service Activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Information and Communication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Financial and Insurance Activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Real Estate Activities and Ownership of Dwellings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Professional, Scientific and Technical Activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Support Service Activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Public Administration and Defence; Compulsory Social Security</t>
+    <t xml:space="preserve">  Tertiary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Wholesale and retail trade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Transport and postal services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Accommodation and food services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Information and communications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Finance and insurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Real estate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Professional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      scientific and technical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Public administration</t>
   </si>
   <si>
     <t xml:space="preserve">    Education</t>
   </si>
   <si>
-    <t xml:space="preserve">    Human Health and Social Work Activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Arts, Entertainment and Recreation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Other Service Activities</t>
-  </si>
-  <si>
-    <t>By Activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Primary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Agriculture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      forestry and fishing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Mining</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Secondary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Electronic components and devices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Fabricated metal products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Basic metal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Food products and beverages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Textile products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Pulp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        paper and paper products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Chemicals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Petroleum and coal products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Non-metallic mineral products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      General-purpose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        production and business oriented machinery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Electrical machinery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        equipment and supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Information and communication electronics equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Transport equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Other manufacturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      gas and water supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        waste management service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Tertiary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Wholesale and retail trade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Transport and postal services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Accommodation and food services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Information and communications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Finance and insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Real estate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Professional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      scientific and technical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Public administration</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Human health and social work</t>
   </si>
   <si>
@@ -466,40 +409,13 @@
   </si>
   <si>
     <t xml:space="preserve">  Sub-total</t>
-  </si>
-  <si>
-    <t>Households</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Saving ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  NGDI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Per capita</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  RGDI</t>
-  </si>
-  <si>
-    <t>HP filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  cycle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  trend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  output gap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -510,13 +426,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -540,16 +449,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1504,7 +1412,7 @@
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D83" s="1">
@@ -1513,362 +1421,362 @@
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="C84" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D84" s="1">
+        <v>21</v>
+      </c>
+      <c r="D84" s="3">
         <v>3.0</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="C85" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D85" s="1">
+        <v>91</v>
+      </c>
+      <c r="D85" s="3">
         <v>3.0</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="C86" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D86" s="1">
+        <v>56</v>
+      </c>
+      <c r="D86" s="3">
         <v>4.0</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="C87" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D87" s="1">
+        <v>92</v>
+      </c>
+      <c r="D87" s="3">
         <v>4.0</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="C88" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D88" s="1">
-        <v>4.0</v>
+        <v>93</v>
+      </c>
+      <c r="D88" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="C89" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D89" s="1">
+        <v>94</v>
+      </c>
+      <c r="D89" s="3">
         <v>4.0</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="C90" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D90" s="1">
-        <v>4.0</v>
+        <v>95</v>
+      </c>
+      <c r="D90" s="3">
+        <v>3.0</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="C91" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D91" s="1">
+        <v>56</v>
+      </c>
+      <c r="D91" s="3">
         <v>4.0</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="C92" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D92" s="1">
+        <v>96</v>
+      </c>
+      <c r="D92" s="3">
         <v>4.0</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="C93" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D93" s="1">
-        <v>4.0</v>
+        <v>63</v>
+      </c>
+      <c r="D93" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="C94" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D94" s="1">
-        <v>4.0</v>
+        <v>97</v>
+      </c>
+      <c r="D94" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="C95" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D95" s="1">
-        <v>4.0</v>
+        <v>98</v>
+      </c>
+      <c r="D95" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="C96" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D96" s="1">
-        <v>4.0</v>
+        <v>99</v>
+      </c>
+      <c r="D96" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="C97" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D97" s="1">
-        <v>4.0</v>
+        <v>100</v>
+      </c>
+      <c r="D97" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="C98" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D98" s="1">
-        <v>4.0</v>
+        <v>101</v>
+      </c>
+      <c r="D98" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="C99" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D99" s="1">
-        <v>4.0</v>
+        <v>102</v>
+      </c>
+      <c r="D99" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="C100" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D100" s="1">
-        <v>4.0</v>
+        <v>103</v>
+      </c>
+      <c r="D100" s="3">
+        <v>6.0</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="C101" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D101" s="1">
-        <v>4.0</v>
+        <v>104</v>
+      </c>
+      <c r="D101" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="C102" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D102" s="1">
-        <v>4.0</v>
+        <v>105</v>
+      </c>
+      <c r="D102" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="C103" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D103" s="1">
-        <v>4.0</v>
+        <v>106</v>
+      </c>
+      <c r="D103" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="C104" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D104" s="1">
-        <v>4.0</v>
+        <v>98</v>
+      </c>
+      <c r="D104" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="C105" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D105" s="1">
-        <v>2.0</v>
+        <v>107</v>
+      </c>
+      <c r="D105" s="3">
+        <v>5.0</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="C106" s="1" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="D106" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="107" ht="15.75" customHeight="1">
+      <c r="C107" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D107" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="108" ht="15.75" customHeight="1">
+      <c r="C108" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D108" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="109" ht="15.75" customHeight="1">
+      <c r="C109" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D109" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="110" ht="15.75" customHeight="1">
+      <c r="C110" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D110" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="111" ht="15.75" customHeight="1">
+      <c r="C111" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D111" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="112" ht="15.75" customHeight="1">
+      <c r="C112" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D112" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="113" ht="15.75" customHeight="1">
+      <c r="C113" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D113" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="114" ht="15.75" customHeight="1">
+      <c r="C114" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D114" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="115" ht="15.75" customHeight="1">
+      <c r="C115" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D115" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="116" ht="15.75" customHeight="1">
+      <c r="C116" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D116" s="3">
         <v>3.0</v>
       </c>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D107" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="1" t="s">
+    <row r="117" ht="15.75" customHeight="1">
+      <c r="C117" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D108" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D109" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D110" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D111" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D112" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D113" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D114" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D115" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D116" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="118" ht="15.75" customHeight="1">
+      <c r="C118" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D117" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="1" t="s">
+      <c r="D118" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="119" ht="15.75" customHeight="1">
+      <c r="C119" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D118" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="120" ht="15.75" customHeight="1">
+      <c r="C120" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D119" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="121" ht="15.75" customHeight="1">
+      <c r="C121" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D120" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="1" t="s">
+      <c r="D121" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="122" ht="15.75" customHeight="1">
+      <c r="C122" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D121" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="1" t="s">
+      <c r="D122" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="123" ht="15.75" customHeight="1">
+      <c r="C123" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D122" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="1" t="s">
+      <c r="D123" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="124" ht="15.75" customHeight="1">
+      <c r="C124" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D123" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="1" t="s">
+      <c r="D124" s="3">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="125" ht="15.75" customHeight="1">
+      <c r="C125" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D124" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="1" t="s">
+      <c r="D125" s="3">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="126" ht="15.75" customHeight="1">
+      <c r="C126" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D125" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="D126" s="3">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="3" t="s">
         <v>128</v>
       </c>
       <c r="D127" s="3">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="1" t="s">
+      <c r="C128" s="3" t="s">
         <v>129</v>
       </c>
       <c r="D128" s="3">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
@@ -1876,7 +1784,7 @@
         <v>130</v>
       </c>
       <c r="D129" s="3">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
@@ -1884,265 +1792,41 @@
         <v>131</v>
       </c>
       <c r="D130" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D131" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D132" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D133" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D134" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D135" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D136" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D137" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D138" s="3">
         <v>3.0</v>
       </c>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D139" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D140" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D141" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D142" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D143" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D144" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D145" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D146" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D147" s="3">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D148" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D149" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D150" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D151" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D152" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D153" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D154" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D155" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D156" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D157" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D158" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D159" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D160" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D161" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D162" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
     <row r="163" ht="15.75" customHeight="1"/>
     <row r="164" ht="15.75" customHeight="1"/>
     <row r="165" ht="15.75" customHeight="1"/>
@@ -2997,7 +2681,7 @@
     <row r="1014" ht="15.75" customHeight="1"/>
     <row r="1015" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="$C$1:$D$162"/>
+  <autoFilter ref="$C$1:$D$130"/>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>

</xml_diff>